<commit_message>
Continued work on CHC identification for Br Ca.
</commit_message>
<xml_diff>
--- a/data/raw/NM-recognition/tmp/Br_Ca_RT_ID_table.xlsx
+++ b/data/raw/NM-recognition/tmp/Br_Ca_RT_ID_table.xlsx
@@ -19,8 +19,77 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="H195" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Could be C28_ene
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H201" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Could be branched alkene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H203" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Could be C29_diene
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J252" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Not same compound
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="340">
   <si>
     <t xml:space="preserve">Peak</t>
   </si>
@@ -736,6 +805,9 @@
     <t xml:space="preserve">P196</t>
   </si>
   <si>
+    <t xml:space="preserve">C28_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P197</t>
   </si>
   <si>
@@ -748,6 +820,9 @@
     <t xml:space="preserve">P200</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_diene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P201</t>
   </si>
   <si>
@@ -757,6 +832,9 @@
     <t xml:space="preserve">P203</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P204</t>
   </si>
   <si>
@@ -766,6 +844,9 @@
     <t xml:space="preserve">P206</t>
   </si>
   <si>
+    <t xml:space="preserve">C29_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P207</t>
   </si>
   <si>
@@ -805,12 +886,18 @@
     <t xml:space="preserve">P219</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_diene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P220</t>
   </si>
   <si>
     <t xml:space="preserve">P221</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P222</t>
   </si>
   <si>
@@ -820,6 +907,9 @@
     <t xml:space="preserve">P224</t>
   </si>
   <si>
+    <t xml:space="preserve">C31_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P225</t>
   </si>
   <si>
@@ -835,6 +925,9 @@
     <t xml:space="preserve">P229</t>
   </si>
   <si>
+    <t xml:space="preserve">C32_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P230</t>
   </si>
   <si>
@@ -853,18 +946,27 @@
     <t xml:space="preserve">P235</t>
   </si>
   <si>
+    <t xml:space="preserve">C33_diene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P236</t>
   </si>
   <si>
     <t xml:space="preserve">P237</t>
   </si>
   <si>
+    <t xml:space="preserve">C33_ene_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P238</t>
   </si>
   <si>
     <t xml:space="preserve">P239</t>
   </si>
   <si>
+    <t xml:space="preserve">C33_ane_NA</t>
+  </si>
+  <si>
     <t xml:space="preserve">P240</t>
   </si>
   <si>
@@ -899,6 +1001,9 @@
   </si>
   <si>
     <t xml:space="preserve">P251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C35_ene_NA</t>
   </si>
   <si>
     <t xml:space="preserve">P252</t>
@@ -1037,12 +1142,24 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7B59"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1079,8 +1196,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1093,6 +1218,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF7B59"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1103,15 +1288,15 @@
   </sheetPr>
   <dimension ref="A1:W287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B190" activeCellId="0" sqref="B190"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="N252" activeCellId="0" sqref="N252"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8730,7 +8915,7 @@
       <c r="G195" s="0" t="n">
         <v>40.178</v>
       </c>
-      <c r="H195" s="0" t="n">
+      <c r="H195" s="1" t="n">
         <v>40.171</v>
       </c>
       <c r="I195" s="0" t="n">
@@ -8800,6 +8985,9 @@
       <c r="A197" s="0" t="s">
         <v>237</v>
       </c>
+      <c r="B197" s="0" t="s">
+        <v>238</v>
+      </c>
       <c r="C197" s="0" t="n">
         <v>40.4438</v>
       </c>
@@ -8866,7 +9054,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C198" s="0" t="n">
         <v>40.743</v>
@@ -8883,7 +9071,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C199" s="0" t="n">
         <v>40.8655789473684</v>
@@ -8948,7 +9136,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C200" s="0" t="n">
         <v>40.943</v>
@@ -8965,7 +9153,10 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>243</v>
       </c>
       <c r="C201" s="0" t="n">
         <v>41.1015294117647</v>
@@ -8982,7 +9173,7 @@
       <c r="G201" s="0" t="n">
         <v>41.108</v>
       </c>
-      <c r="H201" s="0" t="n">
+      <c r="H201" s="1" t="n">
         <v>41.04</v>
       </c>
       <c r="I201" s="0" t="n">
@@ -9024,7 +9215,10 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>243</v>
       </c>
       <c r="C202" s="0" t="n">
         <v>41.1945833333333</v>
@@ -9068,7 +9262,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C203" s="0" t="n">
         <v>41.3054545454545</v>
@@ -9076,7 +9270,7 @@
       <c r="D203" s="0" t="n">
         <v>41.253</v>
       </c>
-      <c r="H203" s="0" t="n">
+      <c r="H203" s="1" t="n">
         <v>41.322</v>
       </c>
       <c r="J203" s="0" t="n">
@@ -9109,7 +9303,10 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>247</v>
       </c>
       <c r="C204" s="0" t="n">
         <v>41.4793333333333</v>
@@ -9153,7 +9350,10 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>247</v>
       </c>
       <c r="C205" s="0" t="n">
         <v>41.5297</v>
@@ -9191,7 +9391,7 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C206" s="0" t="n">
         <v>41.591</v>
@@ -9208,7 +9408,10 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>251</v>
       </c>
       <c r="C207" s="0" t="n">
         <v>41.8154</v>
@@ -9276,7 +9479,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="C208" s="0" t="n">
         <v>42.0716666666667</v>
@@ -9293,7 +9496,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C209" s="0" t="n">
         <v>42.198</v>
@@ -9361,7 +9564,7 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="C210" s="0" t="n">
         <v>42.341</v>
@@ -9381,7 +9584,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C211" s="0" t="n">
         <v>42.4374285714286</v>
@@ -9410,7 +9613,7 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="C212" s="0" t="n">
         <v>42.5702857142857</v>
@@ -9460,7 +9663,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="C213" s="0" t="n">
         <v>42.7255</v>
@@ -9474,7 +9677,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C214" s="0" t="n">
         <v>42.8994666666667</v>
@@ -9527,7 +9730,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C215" s="0" t="n">
         <v>42.9731538461538</v>
@@ -9574,7 +9777,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="C216" s="0" t="n">
         <v>43.0828666666667</v>
@@ -9627,7 +9830,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C217" s="0" t="n">
         <v>43.26875</v>
@@ -9647,7 +9850,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C218" s="0" t="n">
         <v>43.4668888888889</v>
@@ -9682,7 +9885,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C219" s="0" t="n">
         <v>43.6136666666667</v>
@@ -9699,7 +9902,10 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>260</v>
+        <v>264</v>
+      </c>
+      <c r="B220" s="0" t="s">
+        <v>265</v>
       </c>
       <c r="C220" s="0" t="n">
         <v>43.7452352941176</v>
@@ -9758,7 +9964,10 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>261</v>
+        <v>266</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>265</v>
       </c>
       <c r="C221" s="0" t="n">
         <v>43.8401</v>
@@ -9826,7 +10035,10 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>262</v>
+        <v>267</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>268</v>
       </c>
       <c r="C222" s="0" t="n">
         <v>44.0502</v>
@@ -9894,7 +10106,10 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>263</v>
+        <v>269</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>268</v>
       </c>
       <c r="C223" s="0" t="n">
         <v>44.141</v>
@@ -9962,7 +10177,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="C224" s="0" t="n">
         <v>44.24775</v>
@@ -9982,7 +10197,10 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>265</v>
+        <v>271</v>
+      </c>
+      <c r="B225" s="0" t="s">
+        <v>272</v>
       </c>
       <c r="C225" s="0" t="n">
         <v>44.36125</v>
@@ -10050,7 +10268,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C226" s="0" t="n">
         <v>44.7024705882353</v>
@@ -10109,7 +10327,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="C227" s="0" t="n">
         <v>44.8024285714286</v>
@@ -10138,7 +10356,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="C228" s="0" t="n">
         <v>45.0075555555556</v>
@@ -10200,7 +10418,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="C229" s="0" t="n">
         <v>45.1445714285714</v>
@@ -10229,7 +10447,10 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>270</v>
+        <v>277</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>278</v>
       </c>
       <c r="C230" s="0" t="n">
         <v>45.2985</v>
@@ -10279,7 +10500,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="C231" s="0" t="n">
         <v>45.4527</v>
@@ -10317,7 +10538,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="C232" s="0" t="n">
         <v>45.5243157894737</v>
@@ -10382,7 +10603,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="C233" s="0" t="n">
         <v>45.59</v>
@@ -10396,7 +10617,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="C234" s="0" t="n">
         <v>45.7452666666667</v>
@@ -10449,7 +10670,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C235" s="0" t="n">
         <v>45.90525</v>
@@ -10481,7 +10702,10 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>276</v>
+        <v>284</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>285</v>
       </c>
       <c r="C236" s="0" t="n">
         <v>46.2368</v>
@@ -10549,7 +10773,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="C237" s="0" t="n">
         <v>46.349</v>
@@ -10560,7 +10784,10 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>278</v>
+        <v>287</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>288</v>
       </c>
       <c r="C238" s="0" t="n">
         <v>46.5002</v>
@@ -10628,7 +10855,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="C239" s="0" t="n">
         <v>46.6178571428571</v>
@@ -10657,7 +10884,10 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>280</v>
+        <v>290</v>
+      </c>
+      <c r="B240" s="0" t="s">
+        <v>291</v>
       </c>
       <c r="C240" s="0" t="n">
         <v>46.7508421052632</v>
@@ -10722,7 +10952,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="C241" s="0" t="n">
         <v>46.8363333333333</v>
@@ -10739,7 +10969,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="C242" s="0" t="n">
         <v>46.9193571428571</v>
@@ -10789,7 +11019,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="C243" s="0" t="n">
         <v>47.1353684210526</v>
@@ -10854,7 +11084,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="C244" s="0" t="n">
         <v>47.2838571428571</v>
@@ -10883,7 +11113,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="C245" s="0" t="n">
         <v>47.3734</v>
@@ -10936,7 +11166,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="C246" s="0" t="n">
         <v>47.5765</v>
@@ -10980,7 +11210,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
       <c r="C247" s="0" t="n">
         <v>47.6695</v>
@@ -11000,7 +11230,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
       <c r="C248" s="0" t="n">
         <v>47.7754285714286</v>
@@ -11029,7 +11259,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="C249" s="0" t="n">
         <v>47.8712</v>
@@ -11082,7 +11312,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="C250" s="0" t="n">
         <v>47.95725</v>
@@ -11102,7 +11332,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="C251" s="0" t="n">
         <v>48.0975</v>
@@ -11116,7 +11346,10 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>292</v>
+        <v>303</v>
+      </c>
+      <c r="B252" s="0" t="s">
+        <v>304</v>
       </c>
       <c r="C252" s="0" t="n">
         <v>48.49225</v>
@@ -11139,7 +11372,7 @@
       <c r="I252" s="0" t="n">
         <v>48.494</v>
       </c>
-      <c r="J252" s="0" t="n">
+      <c r="J252" s="2" t="n">
         <v>48.48</v>
       </c>
       <c r="K252" s="0" t="n">
@@ -11184,7 +11417,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="C253" s="0" t="n">
         <v>48.5911666666667</v>
@@ -11210,7 +11443,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="C254" s="0" t="n">
         <v>48.70665</v>
@@ -11278,7 +11511,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="C255" s="0" t="n">
         <v>48.8326</v>
@@ -11301,7 +11534,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="C256" s="0" t="n">
         <v>48.9962777777778</v>
@@ -11363,7 +11596,7 @@
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="C257" s="0" t="n">
         <v>49.128</v>
@@ -11386,7 +11619,7 @@
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="C258" s="0" t="n">
         <v>49.204</v>
@@ -11397,7 +11630,7 @@
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="C259" s="0" t="n">
         <v>49.343</v>
@@ -11420,7 +11653,7 @@
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="0" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="C260" s="0" t="n">
         <v>49.452</v>
@@ -11431,7 +11664,7 @@
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="C261" s="0" t="n">
         <v>49.5781</v>
@@ -11469,7 +11702,7 @@
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C262" s="0" t="n">
         <v>49.7035</v>
@@ -11489,7 +11722,7 @@
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="C263" s="0" t="n">
         <v>49.7951666666667</v>
@@ -11533,7 +11766,7 @@
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="C264" s="0" t="n">
         <v>50.038</v>
@@ -11559,7 +11792,7 @@
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="0" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="C265" s="0" t="n">
         <v>50.2007142857143</v>
@@ -11588,7 +11821,7 @@
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="C266" s="0" t="n">
         <v>50.3755625</v>
@@ -11644,7 +11877,7 @@
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="C267" s="0" t="n">
         <v>50.5158666666667</v>
@@ -11697,7 +11930,7 @@
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="C268" s="0" t="n">
         <v>51.0555</v>
@@ -11711,7 +11944,7 @@
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="C269" s="0" t="n">
         <v>51.2723333333333</v>
@@ -11746,7 +11979,7 @@
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="C270" s="0" t="n">
         <v>51.669</v>
@@ -11760,7 +11993,7 @@
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="C271" s="0" t="n">
         <v>51.824</v>
@@ -11771,7 +12004,7 @@
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="C272" s="0" t="n">
         <v>52.065</v>
@@ -11785,7 +12018,7 @@
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="C273" s="0" t="n">
         <v>52.1963333333333</v>
@@ -11811,7 +12044,7 @@
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="C274" s="0" t="n">
         <v>52.3348421052632</v>
@@ -11876,7 +12109,7 @@
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="C275" s="0" t="n">
         <v>52.479</v>
@@ -11896,7 +12129,7 @@
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="C276" s="0" t="n">
         <v>52.6268333333333</v>
@@ -11940,7 +12173,7 @@
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="C277" s="0" t="n">
         <v>53.2975714285714</v>
@@ -11969,7 +12202,7 @@
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="C278" s="0" t="n">
         <v>54.6075</v>
@@ -11995,7 +12228,7 @@
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="C279" s="0" t="n">
         <v>55.01</v>
@@ -12006,7 +12239,7 @@
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="C280" s="0" t="n">
         <v>55.168</v>
@@ -12017,7 +12250,7 @@
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="C281" s="0" t="n">
         <v>55.6615</v>
@@ -12031,7 +12264,7 @@
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="C282" s="0" t="n">
         <v>55.7827</v>
@@ -12069,7 +12302,7 @@
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="C283" s="0" t="n">
         <v>56.16075</v>
@@ -12125,7 +12358,7 @@
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="C284" s="0" t="n">
         <v>56.323</v>
@@ -12145,7 +12378,7 @@
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="C285" s="0" t="n">
         <v>56.7003333333333</v>
@@ -12198,7 +12431,7 @@
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="C286" s="0" t="n">
         <v>57.623</v>
@@ -12209,7 +12442,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="C287" s="0" t="n">
         <v>58.926</v>
@@ -12226,5 +12459,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished identifying CHCs in Br_Ca and begun identifying CHCs in Br_Ib.
</commit_message>
<xml_diff>
--- a/data/raw/NM-recognition/tmp/Br_Ca_RT_ID_table.xlsx
+++ b/data/raw/NM-recognition/tmp/Br_Ca_RT_ID_table.xlsx
@@ -25,6 +25,62 @@
     <author> </author>
   </authors>
   <commentList>
+    <comment ref="D252" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Different compound</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E252" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Other compound overlapping alkadiene</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F252" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Different compound</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G252" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Other compound overlapping alkadiene </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="H195" authorId="0">
       <text>
         <r>
@@ -84,6 +140,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="L252" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Other compound</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M252" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Different compound/noisy</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1003,7 +1087,7 @@
     <t xml:space="preserve">P251</t>
   </si>
   <si>
-    <t xml:space="preserve">C35_ene_NA</t>
+    <t xml:space="preserve">C35_diene_NA</t>
   </si>
   <si>
     <t xml:space="preserve">P252</t>
@@ -1196,7 +1280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1206,6 +1290,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1289,14 +1377,14 @@
   <dimension ref="A1:W287"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N252" activeCellId="0" sqref="N252"/>
+      <selection pane="bottomLeft" activeCell="E255" activeCellId="0" sqref="E255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11354,22 +11442,22 @@
       <c r="C252" s="0" t="n">
         <v>48.49225</v>
       </c>
-      <c r="D252" s="0" t="n">
+      <c r="D252" s="2" t="n">
         <v>48.5</v>
       </c>
-      <c r="E252" s="0" t="n">
+      <c r="E252" s="2" t="n">
         <v>48.5</v>
       </c>
-      <c r="F252" s="0" t="n">
+      <c r="F252" s="2" t="n">
         <v>48.487</v>
       </c>
-      <c r="G252" s="0" t="n">
+      <c r="G252" s="2" t="n">
         <v>48.493</v>
       </c>
       <c r="H252" s="0" t="n">
         <v>48.487</v>
       </c>
-      <c r="I252" s="0" t="n">
+      <c r="I252" s="2" t="n">
         <v>48.494</v>
       </c>
       <c r="J252" s="2" t="n">
@@ -11378,10 +11466,10 @@
       <c r="K252" s="0" t="n">
         <v>48.5</v>
       </c>
-      <c r="L252" s="0" t="n">
+      <c r="L252" s="2" t="n">
         <v>48.487</v>
       </c>
-      <c r="M252" s="0" t="n">
+      <c r="M252" s="2" t="n">
         <v>48.5</v>
       </c>
       <c r="N252" s="0" t="n">
@@ -11445,13 +11533,14 @@
       <c r="A254" s="0" t="s">
         <v>306</v>
       </c>
+      <c r="B254" s="3"/>
       <c r="C254" s="0" t="n">
         <v>48.70665</v>
       </c>
-      <c r="D254" s="0" t="n">
+      <c r="D254" s="3" t="n">
         <v>48.735</v>
       </c>
-      <c r="E254" s="0" t="n">
+      <c r="E254" s="3" t="n">
         <v>48.735</v>
       </c>
       <c r="F254" s="0" t="n">

</xml_diff>

<commit_message>
Begun analysing queeneless hive samples from week 1 and week 3.
</commit_message>
<xml_diff>
--- a/data/raw/NM-recognition/tmp/Br_Ca_RT_ID_table.xlsx
+++ b/data/raw/NM-recognition/tmp/Br_Ca_RT_ID_table.xlsx
@@ -1280,7 +1280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1290,10 +1290,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1377,12 +1373,12 @@
   <dimension ref="A1:W287"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E255" activeCellId="0" sqref="E255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.82"/>
   </cols>
@@ -11533,14 +11529,13 @@
       <c r="A254" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="B254" s="3"/>
       <c r="C254" s="0" t="n">
         <v>48.70665</v>
       </c>
-      <c r="D254" s="3" t="n">
+      <c r="D254" s="0" t="n">
         <v>48.735</v>
       </c>
-      <c r="E254" s="3" t="n">
+      <c r="E254" s="0" t="n">
         <v>48.735</v>
       </c>
       <c r="F254" s="0" t="n">

</xml_diff>